<commit_message>
AR and other Changes
</commit_message>
<xml_diff>
--- a/templates/QARSF/RSTK9329-Verify working of buttons on SO Invoice.xlsx
+++ b/templates/QARSF/RSTK9329-Verify working of buttons on SO Invoice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\WS_RSAutomation\rsqasampleproj\templates\QARSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D671AD9-E6E0-48A1-AC4B-D2A944AB324D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193C4E2D-AB28-4719-868B-AF239B1E345E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="761" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="761" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="PickPackShip" sheetId="13" r:id="rId5"/>
     <sheet name="CreateInvoice" sheetId="18" r:id="rId6"/>
     <sheet name="NewInvoice" sheetId="19" r:id="rId7"/>
+    <sheet name="Payments" sheetId="20" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="52">
   <si>
     <t>API Mode</t>
   </si>
@@ -145,13 +146,64 @@
   </si>
   <si>
     <t>UnitPrice_Updated</t>
+  </si>
+  <si>
+    <t>Select Payment Operation</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Sales Invoice Payment</t>
+  </si>
+  <si>
+    <t>Previous Payment Methods</t>
+  </si>
+  <si>
+    <t>-Enter New Card-</t>
+  </si>
+  <si>
+    <t>Credit Card Number</t>
+  </si>
+  <si>
+    <t>4222222222222</t>
+  </si>
+  <si>
+    <t>Security Code CVV2</t>
+  </si>
+  <si>
+    <t>ExpiresMonth</t>
+  </si>
+  <si>
+    <t>ExpiresYear</t>
+  </si>
+  <si>
+    <t>Address 1</t>
+  </si>
+  <si>
+    <t>My Home10</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>PAYPAL</t>
+  </si>
+  <si>
+    <t>PaymentGateway</t>
+  </si>
+  <si>
+    <t>Select Payment Operation Reverse</t>
+  </si>
+  <si>
+    <t>Sales Invoice Payment Reverse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +230,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -199,11 +257,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -991,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421ECACC-A0FA-44B8-A59E-1E5E133FAF71}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,4 +1097,95 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C5C16DE-81DE-44B5-8F21-3DBAF9DDA390}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2">
+        <v>450</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2">
+        <v>291</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2">
+        <v>500001</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>